<commit_message>
Added sales by region
</commit_message>
<xml_diff>
--- a/Toyota.xlsx
+++ b/Toyota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Prasetyo\Documents\FIT3179\DataVisualisation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4CC0DD-C7FC-4654-8080-F6F3A2E26748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D80E13-3194-4003-ADC7-2A291FEBEF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
   </bookViews>
   <sheets>
     <sheet name="Toyota manufactoring plants" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Toyota sales by region" sheetId="2" r:id="rId3"/>
     <sheet name="Copied" sheetId="4" r:id="rId4"/>
     <sheet name="JapanxWW sales" sheetId="5" r:id="rId5"/>
+    <sheet name="Country Sales" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -1749,8 +1750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9704C40C-0F7D-4014-AC73-652A91C7916C}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2459,6 +2460,12 @@
       </c>
     </row>
     <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
       <c r="C42" t="s">
         <v>100</v>
       </c>
@@ -2470,6 +2477,12 @@
       </c>
     </row>
     <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
       <c r="C43" t="s">
         <v>101</v>
       </c>
@@ -2481,6 +2494,12 @@
       </c>
     </row>
     <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
+        <v>65</v>
+      </c>
       <c r="C44" t="s">
         <v>102</v>
       </c>
@@ -2492,6 +2511,12 @@
       </c>
     </row>
     <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
       <c r="C45" t="s">
         <v>103</v>
       </c>
@@ -2503,6 +2528,12 @@
       </c>
     </row>
     <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>65</v>
+      </c>
       <c r="C46" t="s">
         <v>104</v>
       </c>
@@ -2514,6 +2545,12 @@
       </c>
     </row>
     <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
       <c r="C47" t="s">
         <v>105</v>
       </c>
@@ -2525,6 +2562,12 @@
       </c>
     </row>
     <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" t="s">
+        <v>65</v>
+      </c>
       <c r="C48" t="s">
         <v>106</v>
       </c>
@@ -2536,6 +2579,12 @@
       </c>
     </row>
     <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
       <c r="C49" t="s">
         <v>107</v>
       </c>
@@ -3391,8 +3440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E80F1-E7AC-4FA4-9696-138517751CE3}">
   <dimension ref="B2:P44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5430,4 +5479,1228 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7D43B5-2FBB-4C91-A5CF-3D7BD56EA8F8}">
+  <dimension ref="D3:Q42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:17">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>2010</v>
+      </c>
+      <c r="F3" s="20">
+        <v>2011</v>
+      </c>
+      <c r="G3" s="20">
+        <v>2012</v>
+      </c>
+      <c r="H3" s="20">
+        <v>2013</v>
+      </c>
+      <c r="I3" s="20">
+        <v>2014</v>
+      </c>
+      <c r="J3" s="20">
+        <v>2015</v>
+      </c>
+      <c r="K3" s="20">
+        <v>2016</v>
+      </c>
+      <c r="L3" s="20">
+        <v>2017</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" s="20">
+        <v>2019</v>
+      </c>
+      <c r="O3" s="20">
+        <v>2020</v>
+      </c>
+      <c r="P3" s="20">
+        <v>2021</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="4:17">
+      <c r="D4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="21">
+        <v>101527</v>
+      </c>
+      <c r="F4" s="21">
+        <v>104868</v>
+      </c>
+      <c r="G4" s="21">
+        <v>121305</v>
+      </c>
+      <c r="H4" s="21">
+        <v>123984</v>
+      </c>
+      <c r="I4" s="21">
+        <v>123950</v>
+      </c>
+      <c r="J4" s="21">
+        <v>115470</v>
+      </c>
+      <c r="K4" s="21">
+        <v>119731</v>
+      </c>
+      <c r="L4" s="21">
+        <v>123960</v>
+      </c>
+      <c r="M4" s="21">
+        <v>130297</v>
+      </c>
+      <c r="N4" s="21">
+        <v>120122</v>
+      </c>
+      <c r="O4" s="21">
+        <v>89832</v>
+      </c>
+      <c r="P4" s="21">
+        <v>127620</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>125237</v>
+      </c>
+    </row>
+    <row r="5" spans="4:17">
+      <c r="D5" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1811834</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1698021</v>
+      </c>
+      <c r="G5" s="21">
+        <v>2124664</v>
+      </c>
+      <c r="H5" s="21">
+        <v>2227595</v>
+      </c>
+      <c r="I5" s="21">
+        <v>2428390</v>
+      </c>
+      <c r="J5" s="21">
+        <v>2492722</v>
+      </c>
+      <c r="K5" s="21">
+        <v>2413162</v>
+      </c>
+      <c r="L5" s="21">
+        <v>2473940</v>
+      </c>
+      <c r="M5" s="21">
+        <v>2398415</v>
+      </c>
+      <c r="N5" s="21">
+        <v>2335379</v>
+      </c>
+      <c r="O5" s="21">
+        <v>2220260</v>
+      </c>
+      <c r="P5" s="21">
+        <v>2243788</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>2063425</v>
+      </c>
+    </row>
+    <row r="6" spans="4:17">
+      <c r="D6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="21">
+        <v>166488</v>
+      </c>
+      <c r="F6" s="21">
+        <v>166446</v>
+      </c>
+      <c r="G6" s="21">
+        <v>188171</v>
+      </c>
+      <c r="H6" s="21">
+        <v>197639</v>
+      </c>
+      <c r="I6" s="21">
+        <v>203402</v>
+      </c>
+      <c r="J6" s="21">
+        <v>213146</v>
+      </c>
+      <c r="K6" s="21">
+        <v>217353</v>
+      </c>
+      <c r="L6" s="21">
+        <v>226318</v>
+      </c>
+      <c r="M6" s="21">
+        <v>232953</v>
+      </c>
+      <c r="N6" s="21">
+        <v>228449</v>
+      </c>
+      <c r="O6" s="21">
+        <v>198644</v>
+      </c>
+      <c r="P6" s="21">
+        <v>219185</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>204141</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17">
+      <c r="D7" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="21">
+        <v>49202</v>
+      </c>
+      <c r="F7" s="21">
+        <v>48641</v>
+      </c>
+      <c r="G7" s="21">
+        <v>56727</v>
+      </c>
+      <c r="H7" s="21">
+        <v>61606</v>
+      </c>
+      <c r="I7" s="21">
+        <v>73496</v>
+      </c>
+      <c r="J7" s="21">
+        <v>89079</v>
+      </c>
+      <c r="K7" s="21">
+        <v>108240</v>
+      </c>
+      <c r="L7" s="21">
+        <v>105471</v>
+      </c>
+      <c r="M7" s="21">
+        <v>109058</v>
+      </c>
+      <c r="N7" s="21">
+        <v>103876</v>
+      </c>
+      <c r="O7" s="21">
+        <v>74188</v>
+      </c>
+      <c r="P7" s="21">
+        <v>93184</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>96999</v>
+      </c>
+    </row>
+    <row r="8" spans="4:17">
+      <c r="D8" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="21">
+        <v>217374</v>
+      </c>
+      <c r="F8" s="21">
+        <v>187328</v>
+      </c>
+      <c r="G8" s="21">
+        <v>225790</v>
+      </c>
+      <c r="H8" s="21">
+        <v>221759</v>
+      </c>
+      <c r="I8" s="21">
+        <v>211457</v>
+      </c>
+      <c r="J8" s="21">
+        <v>212807</v>
+      </c>
+      <c r="K8" s="21">
+        <v>220728</v>
+      </c>
+      <c r="L8" s="21">
+        <v>229258</v>
+      </c>
+      <c r="M8" s="21">
+        <v>223096</v>
+      </c>
+      <c r="N8" s="21">
+        <v>215720</v>
+      </c>
+      <c r="O8" s="21">
+        <v>220403</v>
+      </c>
+      <c r="P8" s="21">
+        <v>234091</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>221274</v>
+      </c>
+    </row>
+    <row r="9" spans="4:17">
+      <c r="D9" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="21">
+        <v>505593</v>
+      </c>
+      <c r="F9" s="21">
+        <v>481722</v>
+      </c>
+      <c r="G9" s="21">
+        <v>657464</v>
+      </c>
+      <c r="H9" s="21">
+        <v>672636</v>
+      </c>
+      <c r="I9" s="21">
+        <v>699805</v>
+      </c>
+      <c r="J9" s="21">
+        <v>655657</v>
+      </c>
+      <c r="K9" s="21">
+        <v>475892</v>
+      </c>
+      <c r="L9" s="21">
+        <v>405253</v>
+      </c>
+      <c r="M9" s="21">
+        <v>348394</v>
+      </c>
+      <c r="N9" s="21">
+        <v>377220</v>
+      </c>
+      <c r="O9" s="21">
+        <v>280563</v>
+      </c>
+      <c r="P9" s="21">
+        <v>338319</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>409706</v>
+      </c>
+    </row>
+    <row r="10" spans="4:17">
+      <c r="D10" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="21">
+        <v>98614</v>
+      </c>
+      <c r="F10" s="21">
+        <v>96698</v>
+      </c>
+      <c r="G10" s="21">
+        <v>134489</v>
+      </c>
+      <c r="H10" s="21">
+        <v>178095</v>
+      </c>
+      <c r="I10" s="21">
+        <v>201420</v>
+      </c>
+      <c r="J10" s="21">
+        <v>174644</v>
+      </c>
+      <c r="K10" s="21">
+        <v>179640</v>
+      </c>
+      <c r="L10" s="21">
+        <v>196705</v>
+      </c>
+      <c r="M10" s="21">
+        <v>204808</v>
+      </c>
+      <c r="N10" s="21">
+        <v>207211</v>
+      </c>
+      <c r="O10" s="21">
+        <v>131724</v>
+      </c>
+      <c r="P10" s="21">
+        <v>181479</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>192269</v>
+      </c>
+    </row>
+    <row r="11" spans="4:17" ht="30">
+      <c r="D11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="21">
+        <v>33344</v>
+      </c>
+      <c r="F11" s="21">
+        <v>39515</v>
+      </c>
+      <c r="G11" s="21">
+        <v>48959</v>
+      </c>
+      <c r="H11" s="21">
+        <v>58657</v>
+      </c>
+      <c r="I11" s="21">
+        <v>62827</v>
+      </c>
+      <c r="J11" s="21">
+        <v>70554</v>
+      </c>
+      <c r="K11" s="21">
+        <v>82038</v>
+      </c>
+      <c r="L11" s="21">
+        <v>97513</v>
+      </c>
+      <c r="M11" s="21">
+        <v>81234</v>
+      </c>
+      <c r="N11" s="21">
+        <v>53712</v>
+      </c>
+      <c r="O11" s="21">
+        <v>57528</v>
+      </c>
+      <c r="P11" s="21">
+        <v>71134</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>92073</v>
+      </c>
+    </row>
+    <row r="12" spans="4:17">
+      <c r="D12" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="21">
+        <v>96423</v>
+      </c>
+      <c r="F12" s="21">
+        <v>93208</v>
+      </c>
+      <c r="G12" s="21">
+        <v>102209</v>
+      </c>
+      <c r="H12" s="21">
+        <v>109446</v>
+      </c>
+      <c r="I12" s="21">
+        <v>119605</v>
+      </c>
+      <c r="J12" s="21">
+        <v>124272</v>
+      </c>
+      <c r="K12" s="21">
+        <v>123368</v>
+      </c>
+      <c r="L12" s="21">
+        <v>122725</v>
+      </c>
+      <c r="M12" s="21">
+        <v>124642</v>
+      </c>
+      <c r="N12" s="21">
+        <v>125611</v>
+      </c>
+      <c r="O12" s="21">
+        <v>111219</v>
+      </c>
+      <c r="P12" s="21">
+        <v>131886</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>132748</v>
+      </c>
+    </row>
+    <row r="13" spans="4:17">
+      <c r="D13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="21">
+        <v>106331</v>
+      </c>
+      <c r="F13" s="21">
+        <v>139208</v>
+      </c>
+      <c r="G13" s="21">
+        <v>166261</v>
+      </c>
+      <c r="H13" s="21">
+        <v>177673</v>
+      </c>
+      <c r="I13" s="21">
+        <v>172225</v>
+      </c>
+      <c r="J13" s="21">
+        <v>118835</v>
+      </c>
+      <c r="K13" s="21">
+        <v>117472</v>
+      </c>
+      <c r="L13" s="21">
+        <v>119403</v>
+      </c>
+      <c r="M13" s="21">
+        <v>133804</v>
+      </c>
+      <c r="N13" s="21">
+        <v>133777</v>
+      </c>
+      <c r="O13" s="21">
+        <v>110421</v>
+      </c>
+      <c r="P13" s="21">
+        <v>109485</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>3105</v>
+      </c>
+    </row>
+    <row r="14" spans="4:17">
+      <c r="D14" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="21">
+        <v>73137</v>
+      </c>
+      <c r="F14" s="21">
+        <v>70371</v>
+      </c>
+      <c r="G14" s="21">
+        <v>75899</v>
+      </c>
+      <c r="H14" s="21">
+        <v>79969</v>
+      </c>
+      <c r="I14" s="21">
+        <v>77911</v>
+      </c>
+      <c r="J14" s="21">
+        <v>84707</v>
+      </c>
+      <c r="K14" s="21">
+        <v>92439</v>
+      </c>
+      <c r="L14" s="21">
+        <v>98948</v>
+      </c>
+      <c r="M14" s="21">
+        <v>107165</v>
+      </c>
+      <c r="N14" s="21">
+        <v>119105</v>
+      </c>
+      <c r="O14" s="21">
+        <v>110523</v>
+      </c>
+      <c r="P14" s="21">
+        <v>104496</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>124601</v>
+      </c>
+    </row>
+    <row r="15" spans="4:17">
+      <c r="D15" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="21">
+        <v>79085</v>
+      </c>
+      <c r="F15" s="21">
+        <v>63909</v>
+      </c>
+      <c r="G15" s="21">
+        <v>54837</v>
+      </c>
+      <c r="H15" s="21">
+        <v>59720</v>
+      </c>
+      <c r="I15" s="21">
+        <v>65615</v>
+      </c>
+      <c r="J15" s="21">
+        <v>73818</v>
+      </c>
+      <c r="K15" s="21">
+        <v>82509</v>
+      </c>
+      <c r="L15" s="21">
+        <v>90083</v>
+      </c>
+      <c r="M15" s="21">
+        <v>91375</v>
+      </c>
+      <c r="N15" s="21">
+        <v>91911</v>
+      </c>
+      <c r="O15" s="21">
+        <v>88511</v>
+      </c>
+      <c r="P15" s="21">
+        <v>84930</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>109617</v>
+      </c>
+    </row>
+    <row r="16" spans="4:17">
+      <c r="D16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="21">
+        <v>83577</v>
+      </c>
+      <c r="F16" s="21">
+        <v>82802</v>
+      </c>
+      <c r="G16" s="21">
+        <v>78381</v>
+      </c>
+      <c r="H16" s="21">
+        <v>75948</v>
+      </c>
+      <c r="I16" s="21">
+        <v>70693</v>
+      </c>
+      <c r="J16" s="21">
+        <v>69736</v>
+      </c>
+      <c r="K16" s="21">
+        <v>80406</v>
+      </c>
+      <c r="L16" s="21">
+        <v>86889</v>
+      </c>
+      <c r="M16" s="21">
+        <v>87687</v>
+      </c>
+      <c r="N16" s="21">
+        <v>91232</v>
+      </c>
+      <c r="O16" s="21">
+        <v>83384</v>
+      </c>
+      <c r="P16" s="21">
+        <v>81177</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>91605</v>
+      </c>
+    </row>
+    <row r="17" spans="4:17">
+      <c r="D17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="21">
+        <v>45550</v>
+      </c>
+      <c r="F17" s="21">
+        <v>43007</v>
+      </c>
+      <c r="G17" s="21">
+        <v>35080</v>
+      </c>
+      <c r="H17" s="21">
+        <v>40589</v>
+      </c>
+      <c r="I17" s="21">
+        <v>48808</v>
+      </c>
+      <c r="J17" s="21">
+        <v>59010</v>
+      </c>
+      <c r="K17" s="21">
+        <v>65882</v>
+      </c>
+      <c r="L17" s="21">
+        <v>74095</v>
+      </c>
+      <c r="M17" s="21">
+        <v>80618</v>
+      </c>
+      <c r="N17" s="21">
+        <v>79819</v>
+      </c>
+      <c r="O17" s="21">
+        <v>69785</v>
+      </c>
+      <c r="P17" s="21">
+        <v>75412</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>92091</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17" ht="30">
+      <c r="D18" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="21">
+        <v>886442</v>
+      </c>
+      <c r="F18" s="21">
+        <v>898660</v>
+      </c>
+      <c r="G18" s="21">
+        <v>826800</v>
+      </c>
+      <c r="H18" s="21">
+        <v>974764</v>
+      </c>
+      <c r="I18" s="21">
+        <v>1047622</v>
+      </c>
+      <c r="J18" s="21">
+        <v>1201355</v>
+      </c>
+      <c r="K18" s="21">
+        <v>1230777</v>
+      </c>
+      <c r="L18" s="21">
+        <v>1328467</v>
+      </c>
+      <c r="M18" s="21">
+        <v>1510122</v>
+      </c>
+      <c r="N18" s="21">
+        <v>1543628</v>
+      </c>
+      <c r="O18" s="21">
+        <v>2000084</v>
+      </c>
+      <c r="P18" s="21">
+        <v>1915128</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>1875908</v>
+      </c>
+    </row>
+    <row r="19" spans="4:17">
+      <c r="D19" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="21">
+        <v>299557</v>
+      </c>
+      <c r="F19" s="21">
+        <v>326651</v>
+      </c>
+      <c r="G19" s="21">
+        <v>400717</v>
+      </c>
+      <c r="H19" s="21">
+        <v>437995</v>
+      </c>
+      <c r="I19" s="21">
+        <v>363597</v>
+      </c>
+      <c r="J19" s="21">
+        <v>337647</v>
+      </c>
+      <c r="K19" s="21">
+        <v>397442</v>
+      </c>
+      <c r="L19" s="21">
+        <v>364149</v>
+      </c>
+      <c r="M19" s="21">
+        <v>346858</v>
+      </c>
+      <c r="N19" s="21">
+        <v>322873</v>
+      </c>
+      <c r="O19" s="21">
+        <v>171251</v>
+      </c>
+      <c r="P19" s="21">
+        <v>312301</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>336298</v>
+      </c>
+    </row>
+    <row r="20" spans="4:17">
+      <c r="D20" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="21">
+        <v>349757</v>
+      </c>
+      <c r="F20" s="21">
+        <v>317699</v>
+      </c>
+      <c r="G20" s="21">
+        <v>520119</v>
+      </c>
+      <c r="H20" s="21">
+        <v>404457</v>
+      </c>
+      <c r="I20" s="21">
+        <v>312854</v>
+      </c>
+      <c r="J20" s="21">
+        <v>246476</v>
+      </c>
+      <c r="K20" s="21">
+        <v>253333</v>
+      </c>
+      <c r="L20" s="21">
+        <v>245612</v>
+      </c>
+      <c r="M20" s="21">
+        <v>337125</v>
+      </c>
+      <c r="N20" s="21">
+        <v>302295</v>
+      </c>
+      <c r="O20" s="21">
+        <v>244086</v>
+      </c>
+      <c r="P20" s="21">
+        <v>260936</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>286787</v>
+      </c>
+    </row>
+    <row r="21" spans="4:17">
+      <c r="D21" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="21">
+        <v>58359</v>
+      </c>
+      <c r="F21" s="21">
+        <v>53393</v>
+      </c>
+      <c r="G21" s="21">
+        <v>69812</v>
+      </c>
+      <c r="H21" s="21">
+        <v>81354</v>
+      </c>
+      <c r="I21" s="21">
+        <v>111098</v>
+      </c>
+      <c r="J21" s="21">
+        <v>127709</v>
+      </c>
+      <c r="K21" s="21">
+        <v>168919</v>
+      </c>
+      <c r="L21" s="21">
+        <v>177659</v>
+      </c>
+      <c r="M21" s="21">
+        <v>152118</v>
+      </c>
+      <c r="N21" s="21">
+        <v>154153</v>
+      </c>
+      <c r="O21" s="21">
+        <v>107418</v>
+      </c>
+      <c r="P21" s="21">
+        <v>133802</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>182081</v>
+      </c>
+    </row>
+    <row r="22" spans="4:17">
+      <c r="D22" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="21">
+        <v>114988</v>
+      </c>
+      <c r="F22" s="21">
+        <v>117306</v>
+      </c>
+      <c r="G22" s="21">
+        <v>120785</v>
+      </c>
+      <c r="H22" s="21">
+        <v>125328</v>
+      </c>
+      <c r="I22" s="21">
+        <v>143755</v>
+      </c>
+      <c r="J22" s="21">
+        <v>128709</v>
+      </c>
+      <c r="K22" s="21">
+        <v>137175</v>
+      </c>
+      <c r="L22" s="21">
+        <v>129196</v>
+      </c>
+      <c r="M22" s="21">
+        <v>118784</v>
+      </c>
+      <c r="N22" s="21">
+        <v>145347</v>
+      </c>
+      <c r="O22" s="21">
+        <v>152248</v>
+      </c>
+      <c r="P22" s="21">
+        <v>142200</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>143130</v>
+      </c>
+    </row>
+    <row r="23" spans="4:17">
+      <c r="D23" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="21">
+        <v>92936</v>
+      </c>
+      <c r="F23" s="21">
+        <v>90143</v>
+      </c>
+      <c r="G23" s="21">
+        <v>104046</v>
+      </c>
+      <c r="H23" s="21">
+        <v>96786</v>
+      </c>
+      <c r="I23" s="21">
+        <v>95606</v>
+      </c>
+      <c r="J23" s="21">
+        <v>89746</v>
+      </c>
+      <c r="K23" s="21">
+        <v>71317</v>
+      </c>
+      <c r="L23" s="21">
+        <v>66579</v>
+      </c>
+      <c r="M23" s="21">
+        <v>67600</v>
+      </c>
+      <c r="N23" s="21">
+        <v>66727</v>
+      </c>
+      <c r="O23" s="21">
+        <v>65888</v>
+      </c>
+      <c r="P23" s="21">
+        <v>77690</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>103807</v>
+      </c>
+    </row>
+    <row r="24" spans="4:17">
+      <c r="D24" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="21">
+        <v>48456</v>
+      </c>
+      <c r="F24" s="21">
+        <v>47793</v>
+      </c>
+      <c r="G24" s="21">
+        <v>41643</v>
+      </c>
+      <c r="H24" s="21">
+        <v>38385</v>
+      </c>
+      <c r="I24" s="21">
+        <v>48818</v>
+      </c>
+      <c r="J24" s="21">
+        <v>65086</v>
+      </c>
+      <c r="K24" s="21">
+        <v>62668</v>
+      </c>
+      <c r="L24" s="21">
+        <v>61837</v>
+      </c>
+      <c r="M24" s="21">
+        <v>67058</v>
+      </c>
+      <c r="N24" s="21">
+        <v>41294</v>
+      </c>
+      <c r="O24" s="21">
+        <v>46850</v>
+      </c>
+      <c r="P24" s="21">
+        <v>72155</v>
+      </c>
+      <c r="Q24" s="21">
+        <v>44865</v>
+      </c>
+    </row>
+    <row r="25" spans="4:17">
+      <c r="D25" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="21">
+        <v>31677</v>
+      </c>
+      <c r="F25" s="21">
+        <v>27619</v>
+      </c>
+      <c r="G25" s="21">
+        <v>25947</v>
+      </c>
+      <c r="H25" s="21">
+        <v>34341</v>
+      </c>
+      <c r="I25" s="21">
+        <v>44851</v>
+      </c>
+      <c r="J25" s="21">
+        <v>52664</v>
+      </c>
+      <c r="K25" s="21">
+        <v>59974</v>
+      </c>
+      <c r="L25" s="21">
+        <v>59042</v>
+      </c>
+      <c r="M25" s="21">
+        <v>73334</v>
+      </c>
+      <c r="N25" s="21">
+        <v>75376</v>
+      </c>
+      <c r="O25" s="21">
+        <v>71786</v>
+      </c>
+      <c r="P25" s="21">
+        <v>74373</v>
+      </c>
+      <c r="Q25" s="21">
+        <v>87473</v>
+      </c>
+    </row>
+    <row r="26" spans="4:17">
+      <c r="D26" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="21">
+        <v>10769</v>
+      </c>
+      <c r="F26" s="21">
+        <v>10177</v>
+      </c>
+      <c r="G26" s="21">
+        <v>14732</v>
+      </c>
+      <c r="H26" s="21">
+        <v>12851</v>
+      </c>
+      <c r="I26" s="21">
+        <v>14414</v>
+      </c>
+      <c r="J26" s="21">
+        <v>15476</v>
+      </c>
+      <c r="K26" s="21">
+        <v>21818</v>
+      </c>
+      <c r="L26" s="21">
+        <v>26366</v>
+      </c>
+      <c r="M26" s="21">
+        <v>29856</v>
+      </c>
+      <c r="N26" s="21">
+        <v>18584</v>
+      </c>
+      <c r="O26" s="21">
+        <v>15674</v>
+      </c>
+      <c r="P26" s="21">
+        <v>15510</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>16250</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17">
+      <c r="D27" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="21">
+        <v>128266</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>173439</v>
+      </c>
+    </row>
+    <row r="32" spans="4:17">
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+    </row>
+    <row r="33" spans="4:17">
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+    </row>
+    <row r="34" spans="4:17">
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+    </row>
+    <row r="36" spans="4:17">
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+    </row>
+    <row r="37" spans="4:17">
+      <c r="D37" s="20"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+    </row>
+    <row r="39" spans="4:17">
+      <c r="D39" s="20"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+    </row>
+    <row r="40" spans="4:17">
+      <c r="D40" s="20"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+    </row>
+    <row r="42" spans="4:17">
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added stylings in css
</commit_message>
<xml_diff>
--- a/Toyota.xlsx
+++ b/Toyota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Prasetyo\Documents\FIT3179\DataVisualisation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D80E13-3194-4003-ADC7-2A291FEBEF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD96E6D-915E-463F-BD11-81E61C2ED2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="5" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
   </bookViews>
   <sheets>
     <sheet name="Toyota manufactoring plants" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -5483,1096 +5483,1119 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7D43B5-2FBB-4C91-A5CF-3D7BD56EA8F8}">
-  <dimension ref="D3:Q42"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:17">
-      <c r="D3" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
+      <c r="B1">
         <v>2010</v>
       </c>
-      <c r="F3" s="20">
+      <c r="C1" s="20">
         <v>2011</v>
       </c>
-      <c r="G3" s="20">
+      <c r="D1" s="20">
         <v>2012</v>
       </c>
-      <c r="H3" s="20">
+      <c r="E1" s="20">
         <v>2013</v>
       </c>
-      <c r="I3" s="20">
+      <c r="F1" s="20">
         <v>2014</v>
       </c>
-      <c r="J3" s="20">
+      <c r="G1" s="20">
         <v>2015</v>
       </c>
-      <c r="K3" s="20">
+      <c r="H1" s="20">
         <v>2016</v>
       </c>
-      <c r="L3" s="20">
+      <c r="I1" s="20">
         <v>2017</v>
       </c>
-      <c r="M3" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="N3" s="20">
+      <c r="J1" s="20">
+        <v>2018</v>
+      </c>
+      <c r="K1" s="20">
         <v>2019</v>
       </c>
-      <c r="O3" s="20">
+      <c r="L1" s="20">
         <v>2020</v>
       </c>
-      <c r="P3" s="20">
+      <c r="M1" s="20">
         <v>2021</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="N1" s="20">
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="4:17">
-      <c r="D4" s="20" t="s">
+    <row r="2" spans="1:14" ht="30">
+      <c r="A2" s="20" t="s">
         <v>45</v>
       </c>
+      <c r="B2" s="21">
+        <v>101527</v>
+      </c>
+      <c r="C2" s="21">
+        <v>104868</v>
+      </c>
+      <c r="D2" s="21">
+        <v>121305</v>
+      </c>
+      <c r="E2" s="21">
+        <v>123984</v>
+      </c>
+      <c r="F2" s="21">
+        <v>123950</v>
+      </c>
+      <c r="G2" s="21">
+        <v>115470</v>
+      </c>
+      <c r="H2" s="21">
+        <v>119731</v>
+      </c>
+      <c r="I2" s="21">
+        <v>123960</v>
+      </c>
+      <c r="J2" s="21">
+        <v>130297</v>
+      </c>
+      <c r="K2" s="21">
+        <v>120122</v>
+      </c>
+      <c r="L2" s="21">
+        <v>89832</v>
+      </c>
+      <c r="M2" s="21">
+        <v>127620</v>
+      </c>
+      <c r="N2" s="21">
+        <v>125237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="45">
+      <c r="A3" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="21">
+        <v>1811834</v>
+      </c>
+      <c r="C3" s="21">
+        <v>1698021</v>
+      </c>
+      <c r="D3" s="21">
+        <v>2124664</v>
+      </c>
+      <c r="E3" s="21">
+        <v>2227595</v>
+      </c>
+      <c r="F3" s="21">
+        <v>2428390</v>
+      </c>
+      <c r="G3" s="21">
+        <v>2492722</v>
+      </c>
+      <c r="H3" s="21">
+        <v>2413162</v>
+      </c>
+      <c r="I3" s="21">
+        <v>2473940</v>
+      </c>
+      <c r="J3" s="21">
+        <v>2398415</v>
+      </c>
+      <c r="K3" s="21">
+        <v>2335379</v>
+      </c>
+      <c r="L3" s="21">
+        <v>2220260</v>
+      </c>
+      <c r="M3" s="21">
+        <v>2243788</v>
+      </c>
+      <c r="N3" s="21">
+        <v>2063425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="21">
+        <v>166488</v>
+      </c>
+      <c r="C4" s="21">
+        <v>166446</v>
+      </c>
+      <c r="D4" s="21">
+        <v>188171</v>
+      </c>
       <c r="E4" s="21">
-        <v>101527</v>
+        <v>197639</v>
       </c>
       <c r="F4" s="21">
-        <v>104868</v>
+        <v>203402</v>
       </c>
       <c r="G4" s="21">
-        <v>121305</v>
+        <v>213146</v>
       </c>
       <c r="H4" s="21">
-        <v>123984</v>
+        <v>217353</v>
       </c>
       <c r="I4" s="21">
-        <v>123950</v>
+        <v>226318</v>
       </c>
       <c r="J4" s="21">
-        <v>115470</v>
+        <v>232953</v>
       </c>
       <c r="K4" s="21">
-        <v>119731</v>
+        <v>228449</v>
       </c>
       <c r="L4" s="21">
-        <v>123960</v>
+        <v>198644</v>
       </c>
       <c r="M4" s="21">
-        <v>130297</v>
+        <v>219185</v>
       </c>
       <c r="N4" s="21">
-        <v>120122</v>
-      </c>
-      <c r="O4" s="21">
-        <v>89832</v>
-      </c>
-      <c r="P4" s="21">
-        <v>127620</v>
-      </c>
-      <c r="Q4" s="21">
-        <v>125237</v>
-      </c>
-    </row>
-    <row r="5" spans="4:17">
-      <c r="D5" s="20" t="s">
-        <v>69</v>
+        <v>204141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="21">
+        <v>49202</v>
+      </c>
+      <c r="C5" s="21">
+        <v>48641</v>
+      </c>
+      <c r="D5" s="21">
+        <v>56727</v>
       </c>
       <c r="E5" s="21">
-        <v>1811834</v>
+        <v>61606</v>
       </c>
       <c r="F5" s="21">
-        <v>1698021</v>
+        <v>73496</v>
       </c>
       <c r="G5" s="21">
-        <v>2124664</v>
+        <v>89079</v>
       </c>
       <c r="H5" s="21">
-        <v>2227595</v>
+        <v>108240</v>
       </c>
       <c r="I5" s="21">
-        <v>2428390</v>
+        <v>105471</v>
       </c>
       <c r="J5" s="21">
-        <v>2492722</v>
+        <v>109058</v>
       </c>
       <c r="K5" s="21">
-        <v>2413162</v>
+        <v>103876</v>
       </c>
       <c r="L5" s="21">
-        <v>2473940</v>
+        <v>74188</v>
       </c>
       <c r="M5" s="21">
-        <v>2398415</v>
+        <v>93184</v>
       </c>
       <c r="N5" s="21">
-        <v>2335379</v>
-      </c>
-      <c r="O5" s="21">
-        <v>2220260</v>
-      </c>
-      <c r="P5" s="21">
-        <v>2243788</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>2063425</v>
-      </c>
-    </row>
-    <row r="6" spans="4:17">
-      <c r="D6" s="20" t="s">
-        <v>17</v>
+        <v>96999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="21">
+        <v>217374</v>
+      </c>
+      <c r="C6" s="21">
+        <v>187328</v>
+      </c>
+      <c r="D6" s="21">
+        <v>225790</v>
       </c>
       <c r="E6" s="21">
-        <v>166488</v>
+        <v>221759</v>
       </c>
       <c r="F6" s="21">
-        <v>166446</v>
+        <v>211457</v>
       </c>
       <c r="G6" s="21">
-        <v>188171</v>
+        <v>212807</v>
       </c>
       <c r="H6" s="21">
-        <v>197639</v>
+        <v>220728</v>
       </c>
       <c r="I6" s="21">
-        <v>203402</v>
+        <v>229258</v>
       </c>
       <c r="J6" s="21">
-        <v>213146</v>
+        <v>223096</v>
       </c>
       <c r="K6" s="21">
-        <v>217353</v>
+        <v>215720</v>
       </c>
       <c r="L6" s="21">
-        <v>226318</v>
+        <v>220403</v>
       </c>
       <c r="M6" s="21">
-        <v>232953</v>
+        <v>234091</v>
       </c>
       <c r="N6" s="21">
-        <v>228449</v>
-      </c>
-      <c r="O6" s="21">
-        <v>198644</v>
-      </c>
-      <c r="P6" s="21">
-        <v>219185</v>
-      </c>
-      <c r="Q6" s="21">
-        <v>204141</v>
-      </c>
-    </row>
-    <row r="7" spans="4:17">
-      <c r="D7" s="20" t="s">
-        <v>20</v>
+        <v>221274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="21">
+        <v>505593</v>
+      </c>
+      <c r="C7" s="21">
+        <v>481722</v>
+      </c>
+      <c r="D7" s="21">
+        <v>657464</v>
       </c>
       <c r="E7" s="21">
-        <v>49202</v>
+        <v>672636</v>
       </c>
       <c r="F7" s="21">
-        <v>48641</v>
+        <v>699805</v>
       </c>
       <c r="G7" s="21">
-        <v>56727</v>
+        <v>655657</v>
       </c>
       <c r="H7" s="21">
-        <v>61606</v>
+        <v>475892</v>
       </c>
       <c r="I7" s="21">
-        <v>73496</v>
+        <v>405253</v>
       </c>
       <c r="J7" s="21">
-        <v>89079</v>
+        <v>348394</v>
       </c>
       <c r="K7" s="21">
-        <v>108240</v>
+        <v>377220</v>
       </c>
       <c r="L7" s="21">
-        <v>105471</v>
+        <v>280563</v>
       </c>
       <c r="M7" s="21">
-        <v>109058</v>
+        <v>338319</v>
       </c>
       <c r="N7" s="21">
-        <v>103876</v>
-      </c>
-      <c r="O7" s="21">
-        <v>74188</v>
-      </c>
-      <c r="P7" s="21">
-        <v>93184</v>
-      </c>
-      <c r="Q7" s="21">
-        <v>96999</v>
-      </c>
-    </row>
-    <row r="8" spans="4:17">
-      <c r="D8" s="20" t="s">
-        <v>66</v>
+        <v>409706</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="21">
+        <v>98614</v>
+      </c>
+      <c r="C8" s="21">
+        <v>96698</v>
+      </c>
+      <c r="D8" s="21">
+        <v>134489</v>
       </c>
       <c r="E8" s="21">
-        <v>217374</v>
+        <v>178095</v>
       </c>
       <c r="F8" s="21">
-        <v>187328</v>
+        <v>201420</v>
       </c>
       <c r="G8" s="21">
-        <v>225790</v>
+        <v>174644</v>
       </c>
       <c r="H8" s="21">
-        <v>221759</v>
+        <v>179640</v>
       </c>
       <c r="I8" s="21">
-        <v>211457</v>
+        <v>196705</v>
       </c>
       <c r="J8" s="21">
-        <v>212807</v>
+        <v>204808</v>
       </c>
       <c r="K8" s="21">
-        <v>220728</v>
+        <v>207211</v>
       </c>
       <c r="L8" s="21">
-        <v>229258</v>
+        <v>131724</v>
       </c>
       <c r="M8" s="21">
-        <v>223096</v>
+        <v>181479</v>
       </c>
       <c r="N8" s="21">
-        <v>215720</v>
-      </c>
-      <c r="O8" s="21">
-        <v>220403</v>
-      </c>
-      <c r="P8" s="21">
-        <v>234091</v>
-      </c>
-      <c r="Q8" s="21">
-        <v>221274</v>
-      </c>
-    </row>
-    <row r="9" spans="4:17">
-      <c r="D9" s="20" t="s">
-        <v>80</v>
+        <v>192269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30">
+      <c r="A9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="21">
+        <v>33344</v>
+      </c>
+      <c r="C9" s="21">
+        <v>39515</v>
+      </c>
+      <c r="D9" s="21">
+        <v>48959</v>
       </c>
       <c r="E9" s="21">
-        <v>505593</v>
+        <v>58657</v>
       </c>
       <c r="F9" s="21">
-        <v>481722</v>
+        <v>62827</v>
       </c>
       <c r="G9" s="21">
-        <v>657464</v>
+        <v>70554</v>
       </c>
       <c r="H9" s="21">
-        <v>672636</v>
+        <v>82038</v>
       </c>
       <c r="I9" s="21">
-        <v>699805</v>
+        <v>97513</v>
       </c>
       <c r="J9" s="21">
-        <v>655657</v>
+        <v>81234</v>
       </c>
       <c r="K9" s="21">
-        <v>475892</v>
+        <v>53712</v>
       </c>
       <c r="L9" s="21">
-        <v>405253</v>
+        <v>57528</v>
       </c>
       <c r="M9" s="21">
-        <v>348394</v>
+        <v>71134</v>
       </c>
       <c r="N9" s="21">
-        <v>377220</v>
-      </c>
-      <c r="O9" s="21">
-        <v>280563</v>
-      </c>
-      <c r="P9" s="21">
-        <v>338319</v>
-      </c>
-      <c r="Q9" s="21">
-        <v>409706</v>
-      </c>
-    </row>
-    <row r="10" spans="4:17">
-      <c r="D10" s="20" t="s">
-        <v>24</v>
+        <v>92073</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="21">
+        <v>96423</v>
+      </c>
+      <c r="C10" s="21">
+        <v>93208</v>
+      </c>
+      <c r="D10" s="21">
+        <v>102209</v>
       </c>
       <c r="E10" s="21">
-        <v>98614</v>
+        <v>109446</v>
       </c>
       <c r="F10" s="21">
-        <v>96698</v>
+        <v>119605</v>
       </c>
       <c r="G10" s="21">
-        <v>134489</v>
+        <v>124272</v>
       </c>
       <c r="H10" s="21">
-        <v>178095</v>
+        <v>123368</v>
       </c>
       <c r="I10" s="21">
-        <v>201420</v>
+        <v>122725</v>
       </c>
       <c r="J10" s="21">
-        <v>174644</v>
+        <v>124642</v>
       </c>
       <c r="K10" s="21">
-        <v>179640</v>
+        <v>125611</v>
       </c>
       <c r="L10" s="21">
-        <v>196705</v>
+        <v>111219</v>
       </c>
       <c r="M10" s="21">
-        <v>204808</v>
+        <v>131886</v>
       </c>
       <c r="N10" s="21">
-        <v>207211</v>
-      </c>
-      <c r="O10" s="21">
-        <v>131724</v>
-      </c>
-      <c r="P10" s="21">
-        <v>181479</v>
-      </c>
-      <c r="Q10" s="21">
-        <v>192269</v>
-      </c>
-    </row>
-    <row r="11" spans="4:17" ht="30">
-      <c r="D11" s="20" t="s">
-        <v>23</v>
+        <v>132748</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="21">
+        <v>106331</v>
+      </c>
+      <c r="C11" s="21">
+        <v>139208</v>
+      </c>
+      <c r="D11" s="21">
+        <v>166261</v>
       </c>
       <c r="E11" s="21">
-        <v>33344</v>
+        <v>177673</v>
       </c>
       <c r="F11" s="21">
-        <v>39515</v>
+        <v>172225</v>
       </c>
       <c r="G11" s="21">
-        <v>48959</v>
+        <v>118835</v>
       </c>
       <c r="H11" s="21">
-        <v>58657</v>
+        <v>117472</v>
       </c>
       <c r="I11" s="21">
-        <v>62827</v>
+        <v>119403</v>
       </c>
       <c r="J11" s="21">
-        <v>70554</v>
+        <v>133804</v>
       </c>
       <c r="K11" s="21">
-        <v>82038</v>
+        <v>133777</v>
       </c>
       <c r="L11" s="21">
-        <v>97513</v>
+        <v>110421</v>
       </c>
       <c r="M11" s="21">
-        <v>81234</v>
+        <v>109485</v>
       </c>
       <c r="N11" s="21">
-        <v>53712</v>
-      </c>
-      <c r="O11" s="21">
-        <v>57528</v>
-      </c>
-      <c r="P11" s="21">
-        <v>71134</v>
-      </c>
-      <c r="Q11" s="21">
-        <v>92073</v>
-      </c>
-    </row>
-    <row r="12" spans="4:17">
-      <c r="D12" s="20" t="s">
-        <v>71</v>
+        <v>3105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="21">
+        <v>73137</v>
+      </c>
+      <c r="C12" s="21">
+        <v>70371</v>
+      </c>
+      <c r="D12" s="21">
+        <v>75899</v>
       </c>
       <c r="E12" s="21">
-        <v>96423</v>
+        <v>79969</v>
       </c>
       <c r="F12" s="21">
-        <v>93208</v>
+        <v>77911</v>
       </c>
       <c r="G12" s="21">
-        <v>102209</v>
+        <v>84707</v>
       </c>
       <c r="H12" s="21">
-        <v>109446</v>
+        <v>92439</v>
       </c>
       <c r="I12" s="21">
-        <v>119605</v>
+        <v>98948</v>
       </c>
       <c r="J12" s="21">
-        <v>124272</v>
+        <v>107165</v>
       </c>
       <c r="K12" s="21">
-        <v>123368</v>
+        <v>119105</v>
       </c>
       <c r="L12" s="21">
-        <v>122725</v>
+        <v>110523</v>
       </c>
       <c r="M12" s="21">
-        <v>124642</v>
+        <v>104496</v>
       </c>
       <c r="N12" s="21">
-        <v>125611</v>
-      </c>
-      <c r="O12" s="21">
-        <v>111219</v>
-      </c>
-      <c r="P12" s="21">
-        <v>131886</v>
-      </c>
-      <c r="Q12" s="21">
-        <v>132748</v>
-      </c>
-    </row>
-    <row r="13" spans="4:17">
-      <c r="D13" s="20" t="s">
-        <v>38</v>
+        <v>124601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="21">
+        <v>79085</v>
+      </c>
+      <c r="C13" s="21">
+        <v>63909</v>
+      </c>
+      <c r="D13" s="21">
+        <v>54837</v>
       </c>
       <c r="E13" s="21">
-        <v>106331</v>
+        <v>59720</v>
       </c>
       <c r="F13" s="21">
-        <v>139208</v>
+        <v>65615</v>
       </c>
       <c r="G13" s="21">
-        <v>166261</v>
+        <v>73818</v>
       </c>
       <c r="H13" s="21">
-        <v>177673</v>
+        <v>82509</v>
       </c>
       <c r="I13" s="21">
-        <v>172225</v>
+        <v>90083</v>
       </c>
       <c r="J13" s="21">
-        <v>118835</v>
+        <v>91375</v>
       </c>
       <c r="K13" s="21">
-        <v>117472</v>
+        <v>91911</v>
       </c>
       <c r="L13" s="21">
-        <v>119403</v>
+        <v>88511</v>
       </c>
       <c r="M13" s="21">
-        <v>133804</v>
+        <v>84930</v>
       </c>
       <c r="N13" s="21">
-        <v>133777</v>
-      </c>
-      <c r="O13" s="21">
-        <v>110421</v>
-      </c>
-      <c r="P13" s="21">
-        <v>109485</v>
-      </c>
-      <c r="Q13" s="21">
-        <v>3105</v>
-      </c>
-    </row>
-    <row r="14" spans="4:17">
-      <c r="D14" s="20" t="s">
-        <v>32</v>
+        <v>109617</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="21">
+        <v>83577</v>
+      </c>
+      <c r="C14" s="21">
+        <v>82802</v>
+      </c>
+      <c r="D14" s="21">
+        <v>78381</v>
       </c>
       <c r="E14" s="21">
-        <v>73137</v>
+        <v>75948</v>
       </c>
       <c r="F14" s="21">
-        <v>70371</v>
+        <v>70693</v>
       </c>
       <c r="G14" s="21">
-        <v>75899</v>
+        <v>69736</v>
       </c>
       <c r="H14" s="21">
-        <v>79969</v>
+        <v>80406</v>
       </c>
       <c r="I14" s="21">
-        <v>77911</v>
+        <v>86889</v>
       </c>
       <c r="J14" s="21">
-        <v>84707</v>
+        <v>87687</v>
       </c>
       <c r="K14" s="21">
-        <v>92439</v>
+        <v>91232</v>
       </c>
       <c r="L14" s="21">
-        <v>98948</v>
+        <v>83384</v>
       </c>
       <c r="M14" s="21">
-        <v>107165</v>
+        <v>81177</v>
       </c>
       <c r="N14" s="21">
-        <v>119105</v>
-      </c>
-      <c r="O14" s="21">
-        <v>110523</v>
-      </c>
-      <c r="P14" s="21">
-        <v>104496</v>
-      </c>
-      <c r="Q14" s="21">
-        <v>124601</v>
-      </c>
-    </row>
-    <row r="15" spans="4:17">
-      <c r="D15" s="20" t="s">
-        <v>72</v>
+        <v>91605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="21">
+        <v>45550</v>
+      </c>
+      <c r="C15" s="21">
+        <v>43007</v>
+      </c>
+      <c r="D15" s="21">
+        <v>35080</v>
       </c>
       <c r="E15" s="21">
-        <v>79085</v>
+        <v>40589</v>
       </c>
       <c r="F15" s="21">
-        <v>63909</v>
+        <v>48808</v>
       </c>
       <c r="G15" s="21">
-        <v>54837</v>
+        <v>59010</v>
       </c>
       <c r="H15" s="21">
-        <v>59720</v>
+        <v>65882</v>
       </c>
       <c r="I15" s="21">
-        <v>65615</v>
+        <v>74095</v>
       </c>
       <c r="J15" s="21">
-        <v>73818</v>
+        <v>80618</v>
       </c>
       <c r="K15" s="21">
-        <v>82509</v>
+        <v>79819</v>
       </c>
       <c r="L15" s="21">
-        <v>90083</v>
+        <v>69785</v>
       </c>
       <c r="M15" s="21">
-        <v>91375</v>
+        <v>75412</v>
       </c>
       <c r="N15" s="21">
-        <v>91911</v>
-      </c>
-      <c r="O15" s="21">
-        <v>88511</v>
-      </c>
-      <c r="P15" s="21">
-        <v>84930</v>
-      </c>
-      <c r="Q15" s="21">
-        <v>109617</v>
-      </c>
-    </row>
-    <row r="16" spans="4:17">
-      <c r="D16" s="20" t="s">
-        <v>73</v>
+        <v>92091</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="27.75" customHeight="1">
+      <c r="A16" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="21">
+        <v>886442</v>
+      </c>
+      <c r="C16" s="21">
+        <v>898660</v>
+      </c>
+      <c r="D16" s="21">
+        <v>826800</v>
       </c>
       <c r="E16" s="21">
-        <v>83577</v>
+        <v>974764</v>
       </c>
       <c r="F16" s="21">
-        <v>82802</v>
+        <v>1047622</v>
       </c>
       <c r="G16" s="21">
-        <v>78381</v>
+        <v>1201355</v>
       </c>
       <c r="H16" s="21">
-        <v>75948</v>
+        <v>1230777</v>
       </c>
       <c r="I16" s="21">
-        <v>70693</v>
+        <v>1328467</v>
       </c>
       <c r="J16" s="21">
-        <v>69736</v>
+        <v>1510122</v>
       </c>
       <c r="K16" s="21">
-        <v>80406</v>
+        <v>1543628</v>
       </c>
       <c r="L16" s="21">
-        <v>86889</v>
+        <v>2000084</v>
       </c>
       <c r="M16" s="21">
-        <v>87687</v>
+        <v>1915128</v>
       </c>
       <c r="N16" s="21">
-        <v>91232</v>
-      </c>
-      <c r="O16" s="21">
-        <v>83384</v>
-      </c>
-      <c r="P16" s="21">
-        <v>81177</v>
-      </c>
-      <c r="Q16" s="21">
-        <v>91605</v>
-      </c>
-    </row>
-    <row r="17" spans="4:17">
-      <c r="D17" s="20" t="s">
-        <v>74</v>
+        <v>1875908</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="30">
+      <c r="A17" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="21">
+        <v>299557</v>
+      </c>
+      <c r="C17" s="21">
+        <v>326651</v>
+      </c>
+      <c r="D17" s="21">
+        <v>400717</v>
       </c>
       <c r="E17" s="21">
-        <v>45550</v>
+        <v>437995</v>
       </c>
       <c r="F17" s="21">
-        <v>43007</v>
+        <v>363597</v>
       </c>
       <c r="G17" s="21">
-        <v>35080</v>
+        <v>337647</v>
       </c>
       <c r="H17" s="21">
-        <v>40589</v>
+        <v>397442</v>
       </c>
       <c r="I17" s="21">
-        <v>48808</v>
+        <v>364149</v>
       </c>
       <c r="J17" s="21">
-        <v>59010</v>
+        <v>346858</v>
       </c>
       <c r="K17" s="21">
-        <v>65882</v>
+        <v>322873</v>
       </c>
       <c r="L17" s="21">
-        <v>74095</v>
+        <v>171251</v>
       </c>
       <c r="M17" s="21">
-        <v>80618</v>
+        <v>312301</v>
       </c>
       <c r="N17" s="21">
-        <v>79819</v>
-      </c>
-      <c r="O17" s="21">
-        <v>69785</v>
-      </c>
-      <c r="P17" s="21">
-        <v>75412</v>
-      </c>
-      <c r="Q17" s="21">
-        <v>92091</v>
-      </c>
-    </row>
-    <row r="18" spans="4:17" ht="30">
-      <c r="D18" s="20" t="s">
-        <v>75</v>
+        <v>336298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="21">
+        <v>349757</v>
+      </c>
+      <c r="C18" s="21">
+        <v>317699</v>
+      </c>
+      <c r="D18" s="21">
+        <v>520119</v>
       </c>
       <c r="E18" s="21">
-        <v>886442</v>
+        <v>404457</v>
       </c>
       <c r="F18" s="21">
-        <v>898660</v>
+        <v>312854</v>
       </c>
       <c r="G18" s="21">
-        <v>826800</v>
+        <v>246476</v>
       </c>
       <c r="H18" s="21">
-        <v>974764</v>
+        <v>253333</v>
       </c>
       <c r="I18" s="21">
-        <v>1047622</v>
+        <v>245612</v>
       </c>
       <c r="J18" s="21">
-        <v>1201355</v>
+        <v>337125</v>
       </c>
       <c r="K18" s="21">
-        <v>1230777</v>
+        <v>302295</v>
       </c>
       <c r="L18" s="21">
-        <v>1328467</v>
+        <v>244086</v>
       </c>
       <c r="M18" s="21">
-        <v>1510122</v>
+        <v>260936</v>
       </c>
       <c r="N18" s="21">
-        <v>1543628</v>
-      </c>
-      <c r="O18" s="21">
-        <v>2000084</v>
-      </c>
-      <c r="P18" s="21">
-        <v>1915128</v>
-      </c>
-      <c r="Q18" s="21">
-        <v>1875908</v>
-      </c>
-    </row>
-    <row r="19" spans="4:17">
-      <c r="D19" s="20" t="s">
-        <v>76</v>
+        <v>286787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="30">
+      <c r="A19" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="21">
+        <v>58359</v>
+      </c>
+      <c r="C19" s="21">
+        <v>53393</v>
+      </c>
+      <c r="D19" s="21">
+        <v>69812</v>
       </c>
       <c r="E19" s="21">
-        <v>299557</v>
+        <v>81354</v>
       </c>
       <c r="F19" s="21">
-        <v>326651</v>
+        <v>111098</v>
       </c>
       <c r="G19" s="21">
-        <v>400717</v>
+        <v>127709</v>
       </c>
       <c r="H19" s="21">
-        <v>437995</v>
+        <v>168919</v>
       </c>
       <c r="I19" s="21">
-        <v>363597</v>
+        <v>177659</v>
       </c>
       <c r="J19" s="21">
-        <v>337647</v>
+        <v>152118</v>
       </c>
       <c r="K19" s="21">
-        <v>397442</v>
+        <v>154153</v>
       </c>
       <c r="L19" s="21">
-        <v>364149</v>
+        <v>107418</v>
       </c>
       <c r="M19" s="21">
-        <v>346858</v>
+        <v>133802</v>
       </c>
       <c r="N19" s="21">
-        <v>322873</v>
-      </c>
-      <c r="O19" s="21">
-        <v>171251</v>
-      </c>
-      <c r="P19" s="21">
-        <v>312301</v>
-      </c>
-      <c r="Q19" s="21">
-        <v>336298</v>
-      </c>
-    </row>
-    <row r="20" spans="4:17">
-      <c r="D20" s="20" t="s">
-        <v>60</v>
+        <v>182081</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="21">
+        <v>114988</v>
+      </c>
+      <c r="C20" s="21">
+        <v>117306</v>
+      </c>
+      <c r="D20" s="21">
+        <v>120785</v>
       </c>
       <c r="E20" s="21">
-        <v>349757</v>
+        <v>125328</v>
       </c>
       <c r="F20" s="21">
-        <v>317699</v>
+        <v>143755</v>
       </c>
       <c r="G20" s="21">
-        <v>520119</v>
+        <v>128709</v>
       </c>
       <c r="H20" s="21">
-        <v>404457</v>
+        <v>137175</v>
       </c>
       <c r="I20" s="21">
-        <v>312854</v>
+        <v>129196</v>
       </c>
       <c r="J20" s="21">
-        <v>246476</v>
+        <v>118784</v>
       </c>
       <c r="K20" s="21">
-        <v>253333</v>
+        <v>145347</v>
       </c>
       <c r="L20" s="21">
-        <v>245612</v>
+        <v>152248</v>
       </c>
       <c r="M20" s="21">
-        <v>337125</v>
+        <v>142200</v>
       </c>
       <c r="N20" s="21">
-        <v>302295</v>
-      </c>
-      <c r="O20" s="21">
-        <v>244086</v>
-      </c>
-      <c r="P20" s="21">
-        <v>260936</v>
-      </c>
-      <c r="Q20" s="21">
-        <v>286787</v>
-      </c>
-    </row>
-    <row r="21" spans="4:17">
-      <c r="D21" s="20" t="s">
-        <v>77</v>
+        <v>143130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="21">
+        <v>92936</v>
+      </c>
+      <c r="C21" s="21">
+        <v>90143</v>
+      </c>
+      <c r="D21" s="21">
+        <v>104046</v>
       </c>
       <c r="E21" s="21">
-        <v>58359</v>
+        <v>96786</v>
       </c>
       <c r="F21" s="21">
-        <v>53393</v>
+        <v>95606</v>
       </c>
       <c r="G21" s="21">
-        <v>69812</v>
+        <v>89746</v>
       </c>
       <c r="H21" s="21">
-        <v>81354</v>
+        <v>71317</v>
       </c>
       <c r="I21" s="21">
-        <v>111098</v>
+        <v>66579</v>
       </c>
       <c r="J21" s="21">
-        <v>127709</v>
+        <v>67600</v>
       </c>
       <c r="K21" s="21">
-        <v>168919</v>
+        <v>66727</v>
       </c>
       <c r="L21" s="21">
-        <v>177659</v>
+        <v>65888</v>
       </c>
       <c r="M21" s="21">
-        <v>152118</v>
+        <v>77690</v>
       </c>
       <c r="N21" s="21">
-        <v>154153</v>
-      </c>
-      <c r="O21" s="21">
-        <v>107418</v>
-      </c>
-      <c r="P21" s="21">
-        <v>133802</v>
-      </c>
-      <c r="Q21" s="21">
-        <v>182081</v>
-      </c>
-    </row>
-    <row r="22" spans="4:17">
-      <c r="D22" s="20" t="s">
-        <v>58</v>
+        <v>103807</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="21">
+        <v>48456</v>
+      </c>
+      <c r="C22" s="21">
+        <v>47793</v>
+      </c>
+      <c r="D22" s="21">
+        <v>41643</v>
       </c>
       <c r="E22" s="21">
-        <v>114988</v>
+        <v>38385</v>
       </c>
       <c r="F22" s="21">
-        <v>117306</v>
+        <v>48818</v>
       </c>
       <c r="G22" s="21">
-        <v>120785</v>
+        <v>65086</v>
       </c>
       <c r="H22" s="21">
-        <v>125328</v>
+        <v>62668</v>
       </c>
       <c r="I22" s="21">
-        <v>143755</v>
+        <v>61837</v>
       </c>
       <c r="J22" s="21">
-        <v>128709</v>
+        <v>67058</v>
       </c>
       <c r="K22" s="21">
-        <v>137175</v>
+        <v>41294</v>
       </c>
       <c r="L22" s="21">
-        <v>129196</v>
+        <v>46850</v>
       </c>
       <c r="M22" s="21">
-        <v>118784</v>
+        <v>72155</v>
       </c>
       <c r="N22" s="21">
-        <v>145347</v>
-      </c>
-      <c r="O22" s="21">
-        <v>152248</v>
-      </c>
-      <c r="P22" s="21">
-        <v>142200</v>
-      </c>
-      <c r="Q22" s="21">
-        <v>143130</v>
-      </c>
-    </row>
-    <row r="23" spans="4:17">
-      <c r="D23" s="20" t="s">
-        <v>61</v>
+        <v>44865</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="21">
+        <v>31677</v>
+      </c>
+      <c r="C23" s="21">
+        <v>27619</v>
+      </c>
+      <c r="D23" s="21">
+        <v>25947</v>
       </c>
       <c r="E23" s="21">
-        <v>92936</v>
+        <v>34341</v>
       </c>
       <c r="F23" s="21">
-        <v>90143</v>
+        <v>44851</v>
       </c>
       <c r="G23" s="21">
-        <v>104046</v>
+        <v>52664</v>
       </c>
       <c r="H23" s="21">
-        <v>96786</v>
+        <v>59974</v>
       </c>
       <c r="I23" s="21">
-        <v>95606</v>
+        <v>59042</v>
       </c>
       <c r="J23" s="21">
-        <v>89746</v>
+        <v>73334</v>
       </c>
       <c r="K23" s="21">
-        <v>71317</v>
+        <v>75376</v>
       </c>
       <c r="L23" s="21">
-        <v>66579</v>
+        <v>71786</v>
       </c>
       <c r="M23" s="21">
-        <v>67600</v>
+        <v>74373</v>
       </c>
       <c r="N23" s="21">
-        <v>66727</v>
-      </c>
-      <c r="O23" s="21">
-        <v>65888</v>
-      </c>
-      <c r="P23" s="21">
-        <v>77690</v>
-      </c>
-      <c r="Q23" s="21">
-        <v>103807</v>
-      </c>
-    </row>
-    <row r="24" spans="4:17">
-      <c r="D24" s="20" t="s">
-        <v>57</v>
+        <v>87473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="30">
+      <c r="A24" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="21">
+        <v>10769</v>
+      </c>
+      <c r="C24" s="21">
+        <v>10177</v>
+      </c>
+      <c r="D24" s="21">
+        <v>14732</v>
       </c>
       <c r="E24" s="21">
-        <v>48456</v>
+        <v>12851</v>
       </c>
       <c r="F24" s="21">
-        <v>47793</v>
+        <v>14414</v>
       </c>
       <c r="G24" s="21">
-        <v>41643</v>
+        <v>15476</v>
       </c>
       <c r="H24" s="21">
-        <v>38385</v>
+        <v>21818</v>
       </c>
       <c r="I24" s="21">
-        <v>48818</v>
+        <v>26366</v>
       </c>
       <c r="J24" s="21">
-        <v>65086</v>
+        <v>29856</v>
       </c>
       <c r="K24" s="21">
-        <v>62668</v>
+        <v>18584</v>
       </c>
       <c r="L24" s="21">
-        <v>61837</v>
+        <v>15674</v>
       </c>
       <c r="M24" s="21">
-        <v>67058</v>
+        <v>15510</v>
       </c>
       <c r="N24" s="21">
-        <v>41294</v>
-      </c>
-      <c r="O24" s="21">
-        <v>46850</v>
-      </c>
-      <c r="P24" s="21">
-        <v>72155</v>
-      </c>
-      <c r="Q24" s="21">
-        <v>44865</v>
-      </c>
-    </row>
-    <row r="25" spans="4:17">
-      <c r="D25" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="21">
-        <v>31677</v>
-      </c>
-      <c r="F25" s="21">
-        <v>27619</v>
-      </c>
-      <c r="G25" s="21">
-        <v>25947</v>
-      </c>
-      <c r="H25" s="21">
-        <v>34341</v>
-      </c>
-      <c r="I25" s="21">
-        <v>44851</v>
-      </c>
-      <c r="J25" s="21">
-        <v>52664</v>
-      </c>
-      <c r="K25" s="21">
-        <v>59974</v>
-      </c>
-      <c r="L25" s="21">
-        <v>59042</v>
+        <v>16250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="20">
+        <v>0</v>
+      </c>
+      <c r="C25" s="20">
+        <v>0</v>
+      </c>
+      <c r="D25" s="20">
+        <v>0</v>
+      </c>
+      <c r="E25" s="20">
+        <v>0</v>
+      </c>
+      <c r="F25" s="20">
+        <v>0</v>
+      </c>
+      <c r="G25" s="20">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20">
+        <v>0</v>
+      </c>
+      <c r="I25" s="20">
+        <v>0</v>
+      </c>
+      <c r="J25" s="20">
+        <v>0</v>
+      </c>
+      <c r="K25" s="20">
+        <v>0</v>
+      </c>
+      <c r="L25" s="20">
+        <v>0</v>
       </c>
       <c r="M25" s="21">
-        <v>73334</v>
+        <v>128266</v>
       </c>
       <c r="N25" s="21">
-        <v>75376</v>
-      </c>
-      <c r="O25" s="21">
-        <v>71786</v>
-      </c>
-      <c r="P25" s="21">
-        <v>74373</v>
-      </c>
-      <c r="Q25" s="21">
-        <v>87473</v>
-      </c>
-    </row>
-    <row r="26" spans="4:17">
-      <c r="D26" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="21">
-        <v>10769</v>
-      </c>
-      <c r="F26" s="21">
-        <v>10177</v>
-      </c>
-      <c r="G26" s="21">
-        <v>14732</v>
-      </c>
-      <c r="H26" s="21">
-        <v>12851</v>
-      </c>
-      <c r="I26" s="21">
-        <v>14414</v>
-      </c>
-      <c r="J26" s="21">
-        <v>15476</v>
-      </c>
-      <c r="K26" s="21">
-        <v>21818</v>
-      </c>
-      <c r="L26" s="21">
-        <v>26366</v>
-      </c>
-      <c r="M26" s="21">
-        <v>29856</v>
-      </c>
-      <c r="N26" s="21">
-        <v>18584</v>
-      </c>
-      <c r="O26" s="21">
-        <v>15674</v>
-      </c>
-      <c r="P26" s="21">
-        <v>15510</v>
-      </c>
-      <c r="Q26" s="21">
-        <v>16250</v>
-      </c>
-    </row>
-    <row r="27" spans="4:17">
-      <c r="D27" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="21">
-        <v>128266</v>
-      </c>
-      <c r="Q27" s="21">
         <v>173439</v>
       </c>
     </row>
-    <row r="32" spans="4:17">
+    <row r="32" spans="1:17">
       <c r="D32" s="20"/>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>

</xml_diff>

<commit_message>
Initialised Layout for graphs
</commit_message>
<xml_diff>
--- a/Toyota.xlsx
+++ b/Toyota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Prasetyo\Documents\FIT3179\DataVisualisation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD96E6D-915E-463F-BD11-81E61C2ED2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEC9CC2-8ECE-425A-9145-78CD74032C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="5" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
   </bookViews>
   <sheets>
     <sheet name="Toyota manufactoring plants" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Copied" sheetId="4" r:id="rId4"/>
     <sheet name="JapanxWW sales" sheetId="5" r:id="rId5"/>
     <sheet name="Country Sales" sheetId="6" r:id="rId6"/>
+    <sheet name="Best selling cars in 2022 ww" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -360,6 +361,63 @@
   </si>
   <si>
     <t>Toyota Motor Corporation Australia Ltd. (TMCA)</t>
+  </si>
+  <si>
+    <t>Toyota Corolla</t>
+  </si>
+  <si>
+    <t>Toyota RAV4</t>
+  </si>
+  <si>
+    <t>Ford F-Series</t>
+  </si>
+  <si>
+    <t>Tesla Model Y</t>
+  </si>
+  <si>
+    <t>Toyota Camry</t>
+  </si>
+  <si>
+    <t>Honda CR-V</t>
+  </si>
+  <si>
+    <t>Tesla Model 3</t>
+  </si>
+  <si>
+    <t>Chevy Silverado</t>
+  </si>
+  <si>
+    <t>Toyota Hilux</t>
+  </si>
+  <si>
+    <t>Hyundai Tucson</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Units Sold</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>Chervolet</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9704C40C-0F7D-4014-AC73-652A91C7916C}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
@@ -3441,7 +3499,7 @@
   <dimension ref="B2:P44"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:P41"/>
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5485,7 +5543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7D43B5-2FBB-4C91-A5CF-3D7BD56EA8F8}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -5539,7 +5597,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30">
+    <row r="2" spans="1:14">
       <c r="A2" s="20" t="s">
         <v>45</v>
       </c>
@@ -5583,7 +5641,7 @@
         <v>125237</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="45">
+    <row r="3" spans="1:14">
       <c r="A3" s="20" t="s">
         <v>69</v>
       </c>
@@ -5847,7 +5905,7 @@
         <v>192269</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30">
+    <row r="9" spans="1:14">
       <c r="A9" s="20" t="s">
         <v>23</v>
       </c>
@@ -6199,7 +6257,7 @@
         <v>1875908</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="30">
+    <row r="17" spans="1:17">
       <c r="A17" s="20" t="s">
         <v>76</v>
       </c>
@@ -6287,7 +6345,7 @@
         <v>286787</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="30">
+    <row r="19" spans="1:17">
       <c r="A19" s="20" t="s">
         <v>77</v>
       </c>
@@ -6507,7 +6565,7 @@
         <v>87473</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="30">
+    <row r="24" spans="1:17">
       <c r="A24" s="20" t="s">
         <v>78</v>
       </c>
@@ -6726,4 +6784,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5EAB2D-9342-4DBC-968C-4DBB7D82EB7F}">
+  <dimension ref="A2:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>1120000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4">
+        <v>870000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5">
+        <v>787000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6">
+        <v>786000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7">
+        <v>675000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8">
+        <v>601000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9">
+        <v>596000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10">
+        <v>592000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11">
+        <v>564000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12">
+        <v>564000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added pictures to be used in top10cars
</commit_message>
<xml_diff>
--- a/Toyota.xlsx
+++ b/Toyota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Prasetyo\Documents\FIT3179\DataVisualisation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D3FD0599-F43B-4ABF-8FCB-7E270932DB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56785230-A275-4DB9-85B7-08F8C3DDEADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="6" activeTab="7" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="6" activeTab="8" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
   </bookViews>
   <sheets>
     <sheet name="Toyota manufactoring plants" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="152">
   <si>
     <t>Name</t>
   </si>
@@ -401,9 +401,6 @@
     <t>Brand</t>
   </si>
   <si>
-    <t>Units Sold</t>
-  </si>
-  <si>
     <t>Toyota</t>
   </si>
   <si>
@@ -456,6 +453,42 @@
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>UnitsSold</t>
+  </si>
+  <si>
+    <t>"images/Car/corolla.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/rav4.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/camry.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/silverado.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/hilux.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/tucson.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/fseries.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/modely.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/model3.png"</t>
+  </si>
+  <si>
+    <t>"images/Car/crv.png</t>
   </si>
 </sst>
 </file>
@@ -5644,7 +5677,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="19">
         <v>1811834</v>
@@ -5973,7 +6006,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="19">
         <v>96423</v>
@@ -6678,7 +6711,7 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="19">
         <v>10769</v>
@@ -6913,7 +6946,7 @@
         <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C29" s="19">
         <v>29573</v>
@@ -6960,7 +6993,7 @@
         <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C30" s="19">
         <v>505593</v>
@@ -7248,7 +7281,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="19">
         <v>945432</v>
@@ -7530,7 +7563,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="19">
         <v>136927</v>
@@ -7718,7 +7751,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" s="19">
         <v>82920</v>
@@ -7765,7 +7798,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -8235,7 +8268,7 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -8564,7 +8597,7 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -8612,7 +8645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31CFB4A-BA25-46C8-9C19-268C11915BF8}">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -8631,7 +8664,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D1">
         <v>2010</v>
@@ -8678,10 +8711,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="23">
         <v>945432</v>
@@ -8731,7 +8764,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="23">
         <v>458592</v>
@@ -8781,7 +8814,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" s="23">
         <v>54048</v>
@@ -8831,7 +8864,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="23">
         <v>66237</v>
@@ -8881,7 +8914,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" s="23">
         <v>69950</v>
@@ -8931,7 +8964,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7" s="23">
         <v>14061</v>
@@ -8978,10 +9011,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" s="23">
         <v>136927</v>
@@ -9031,7 +9064,7 @@
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="23">
         <v>83384</v>
@@ -9081,7 +9114,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" s="23">
         <v>158504</v>
@@ -9131,7 +9164,7 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" s="23">
         <v>0</v>
@@ -9178,10 +9211,10 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D12" s="23">
         <v>82920</v>
@@ -9228,10 +9261,10 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" s="23">
         <v>0</v>
@@ -9281,7 +9314,7 @@
         <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="23">
         <v>264622</v>
@@ -9331,7 +9364,7 @@
         <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D15" s="23">
         <v>629944</v>
@@ -9381,7 +9414,7 @@
         <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D16" s="23">
         <v>28432</v>
@@ -9431,7 +9464,7 @@
         <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" s="23">
         <v>65137</v>
@@ -9481,7 +9514,7 @@
         <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D18" s="23">
         <v>117696</v>
@@ -9531,7 +9564,7 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" s="23">
         <v>30618</v>
@@ -9581,7 +9614,7 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" s="23">
         <v>75515</v>
@@ -9631,7 +9664,7 @@
         <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D21" s="23">
         <v>769941</v>
@@ -9681,7 +9714,7 @@
         <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22" s="23">
         <v>45577</v>
@@ -9728,10 +9761,10 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D23" s="23">
         <v>0</v>
@@ -9781,7 +9814,7 @@
         <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" s="23">
         <v>3282855</v>
@@ -9831,7 +9864,7 @@
         <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25" s="23">
         <v>119473</v>
@@ -9881,7 +9914,7 @@
         <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D26" s="23">
         <v>123484</v>
@@ -9931,7 +9964,7 @@
         <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D27" s="23">
         <v>123484</v>
@@ -9981,7 +10014,7 @@
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D28" s="23">
         <v>0</v>
@@ -10031,7 +10064,7 @@
         <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D29" s="23">
         <v>0</v>
@@ -10078,10 +10111,10 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D30" s="23">
         <v>0</v>
@@ -10126,10 +10159,10 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D31" s="23">
         <v>1811834</v>
@@ -10179,7 +10212,7 @@
         <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D32" s="23">
         <v>166488</v>
@@ -10229,7 +10262,7 @@
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D33" s="23">
         <v>49202</v>
@@ -10279,7 +10312,7 @@
         <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D34" s="23">
         <v>26163</v>
@@ -10329,7 +10362,7 @@
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D35" s="23">
         <v>98614</v>
@@ -10379,7 +10412,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D36" s="23">
         <v>33344</v>
@@ -10429,7 +10462,7 @@
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D37" s="23">
         <v>142350</v>
@@ -10476,10 +10509,10 @@
         <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" s="23">
         <v>96423</v>
@@ -10529,7 +10562,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D39" s="23">
         <v>106331</v>
@@ -10579,7 +10612,7 @@
         <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D40" s="23">
         <v>73137</v>
@@ -10629,7 +10662,7 @@
         <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D41" s="23">
         <v>79085</v>
@@ -10679,7 +10712,7 @@
         <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D42" s="23">
         <v>83577</v>
@@ -10729,7 +10762,7 @@
         <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D43" s="23">
         <v>45550</v>
@@ -10779,7 +10812,7 @@
         <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D44" s="23">
         <v>329432</v>
@@ -10829,7 +10862,7 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D45" s="23">
         <v>886442</v>
@@ -10879,7 +10912,7 @@
         <v>76</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D46" s="23">
         <v>299557</v>
@@ -10929,7 +10962,7 @@
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" s="23">
         <v>349757</v>
@@ -10979,7 +11012,7 @@
         <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D48" s="23">
         <v>58359</v>
@@ -11029,7 +11062,7 @@
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D49" s="23">
         <v>114988</v>
@@ -11079,7 +11112,7 @@
         <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D50" s="23">
         <v>92936</v>
@@ -11129,7 +11162,7 @@
         <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51" s="23">
         <v>48456</v>
@@ -11179,7 +11212,7 @@
         <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D52" s="23">
         <v>31677</v>
@@ -11226,10 +11259,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D53" s="23">
         <v>10769</v>
@@ -11279,7 +11312,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D54" s="23">
         <v>0</v>
@@ -11329,7 +11362,7 @@
         <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D55" s="23">
         <v>103275</v>
@@ -11379,7 +11412,7 @@
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D56" s="23">
         <v>1407141</v>
@@ -11429,7 +11462,7 @@
         <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D57" s="23">
         <v>217374</v>
@@ -11476,10 +11509,10 @@
         <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D58" s="23">
         <v>29573</v>
@@ -11526,10 +11559,10 @@
         <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" s="23">
         <v>505593</v>
@@ -11579,7 +11612,7 @@
         <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D60" s="23">
         <v>65454</v>
@@ -11629,7 +11662,7 @@
         <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D61" s="23">
         <v>101527</v>
@@ -11679,7 +11712,7 @@
         <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D62" s="23">
         <v>93970</v>
@@ -11728,19 +11761,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5EAB2D-9342-4DBC-968C-4DBB7D82EB7F}">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -11748,12 +11783,15 @@
         <v>120</v>
       </c>
       <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>110</v>
@@ -11761,10 +11799,13 @@
       <c r="C3">
         <v>1120000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
         <v>111</v>
@@ -11772,10 +11813,13 @@
       <c r="C4">
         <v>870000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
         <v>112</v>
@@ -11783,10 +11827,13 @@
       <c r="C5">
         <v>787000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
         <v>113</v>
@@ -11794,10 +11841,13 @@
       <c r="C6">
         <v>786000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>114</v>
@@ -11805,10 +11855,13 @@
       <c r="C7">
         <v>675000</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>115</v>
@@ -11816,10 +11869,13 @@
       <c r="C8">
         <v>601000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
         <v>116</v>
@@ -11827,10 +11883,13 @@
       <c r="C9">
         <v>596000</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
         <v>117</v>
@@ -11838,10 +11897,13 @@
       <c r="C10">
         <v>592000</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
         <v>118</v>
@@ -11849,16 +11911,22 @@
       <c r="C11">
         <v>564000</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
         <v>119</v>
       </c>
       <c r="C12">
         <v>564000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added wilkinson data for wilkinson dot plot for top cars later
</commit_message>
<xml_diff>
--- a/Toyota.xlsx
+++ b/Toyota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Prasetyo\Documents\FIT3179\DataVisualisation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4281DC1A-B911-4489-8805-220A892F90BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF51C6D-87CF-4932-9E86-1513CC2A929C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="12" activeTab="12" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="12" activeTab="13" xr2:uid="{7CCEE7ED-8278-441A-9737-349745DE560B}"/>
   </bookViews>
   <sheets>
     <sheet name="Toyota manufactoring plants" sheetId="1" r:id="rId1"/>
@@ -32124,8 +32124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC0CB14-7CF2-4A1A-B991-4AAFE9DB1F51}">
   <dimension ref="A1:E833"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H775" sqref="H775"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -46305,8 +46305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5EAB2D-9342-4DBC-968C-4DBB7D82EB7F}">
   <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>